<commit_message>
Update application and data handling; enhance type hints, add configuration for VSCode, and modify queue broadcasting
</commit_message>
<xml_diff>
--- a/assets/xlsx_database.xlsx
+++ b/assets/xlsx_database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\86781\VS_Code_Project\form_filler_new\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE993AB-CB65-4A3B-ACEA-B0CC0F7B321B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31140F40-B2D9-4630-9427-D2ACC52FBD03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="93">
   <si>
     <t>姓名</t>
   </si>
@@ -361,6 +361,9 @@
   </si>
   <si>
     <t>简历</t>
+  </si>
+  <si>
+    <t>过往</t>
   </si>
 </sst>
 </file>
@@ -1041,7 +1044,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1170,6 +1173,9 @@
       </c>
       <c r="B10" t="s">
         <v>91</v>
+      </c>
+      <c r="C10" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Refactor configuration handling; update .gitignore, enhance type hints, and improve keyboard service management
</commit_message>
<xml_diff>
--- a/assets/xlsx_database.xlsx
+++ b/assets/xlsx_database.xlsx
@@ -473,11 +473,7 @@
           <t>Name</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>test_name</t>
-        </is>
-      </c>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
@@ -525,7 +521,11 @@
           <t>Sex</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>gender</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>

</xml_diff>

<commit_message>
Update README, enhance backup functionality, and refine .gitignore
</commit_message>
<xml_diff>
--- a/assets/xlsx_database.xlsx
+++ b/assets/xlsx_database.xlsx
@@ -602,7 +602,11 @@
           <t>电子邮件</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>联系方式</t>
+        </is>
+      </c>
       <c r="G7" t="inlineStr"/>
     </row>
     <row r="8">

</xml_diff>